<commit_message>
formulario de pedidos con agregar, mostrar y crear pedidos
</commit_message>
<xml_diff>
--- a/ProyectoPooDist/excels/pedidos_calendario.xlsx
+++ b/ProyectoPooDist/excels/pedidos_calendario.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
   <si>
     <t>Fecha C</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t>2024-10-09</t>
+  </si>
+  <si>
+    <t>2024-10-27</t>
+  </si>
+  <si>
+    <t>2024-10-28</t>
   </si>
 </sst>
 </file>
@@ -107,7 +113,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:L6"/>
+  <dimension ref="A1:N7"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -179,7 +185,7 @@
         <v>6.0</v>
       </c>
       <c r="E3" t="b" s="0">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F3" t="b" s="0">
         <v>0</v>
@@ -297,6 +303,50 @@
       </c>
       <c r="J6" t="n" s="0">
         <v>60.0</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="s" s="0">
+        <v>17</v>
+      </c>
+      <c r="B7" t="s" s="0">
+        <v>18</v>
+      </c>
+      <c r="C7" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="D7" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="E7" t="b" s="0">
+        <v>1</v>
+      </c>
+      <c r="F7" t="b" s="0">
+        <v>1</v>
+      </c>
+      <c r="G7" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="H7" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="I7" t="n" s="0">
+        <v>3.0</v>
+      </c>
+      <c r="J7" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="K7" t="n" s="0">
+        <v>5.0</v>
+      </c>
+      <c r="L7" t="n" s="0">
+        <v>1.0</v>
+      </c>
+      <c r="M7" t="n" s="0">
+        <v>7.0</v>
+      </c>
+      <c r="N7" t="n" s="0">
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>